<commit_message>
cianci_model.m ================ -ve N1 corrected. Sparse time vector.
cianci_pulseTrain.m
=====================
Stopping criteria. 1) Normalized slope < exp(-5)
                   2) First slope = 0

sweep_tau.m
=============
10 ns breakpoint
-------
       \
        \
         \
</commit_message>
<xml_diff>
--- a/sweep tau.xlsx
+++ b/sweep tau.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -322,11 +323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226092792"/>
-        <c:axId val="226092400"/>
+        <c:axId val="201136480"/>
+        <c:axId val="201136864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226092792"/>
+        <c:axId val="201136480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -384,12 +385,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226092400"/>
+        <c:crossAx val="201136864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226092400"/>
+        <c:axId val="201136864"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -447,7 +448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226092792"/>
+        <c:crossAx val="201136480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,7 +1354,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>